<commit_message>
Update Excel data files
</commit_message>
<xml_diff>
--- a/all_hotels_puerto_rico.xlsx
+++ b/all_hotels_puerto_rico.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Foundation for PR\Hotel API\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF1B6337-938E-4DF1-801F-21C5185C71D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A829129-111E-4CAD-8FD2-B03BBF9C44A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-180" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -10061,7 +10061,32 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FFFFFFFF"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF4472C4"/>
+          <bgColor rgb="FF4472C4"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -10072,6 +10097,22 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{298544C3-93B3-418D-8DFE-6284C149C5C6}" name="Tabla1" displayName="Tabla1" ref="A1:G1109" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:G1109" xr:uid="{298544C3-93B3-418D-8DFE-6284C149C5C6}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{6A78BADA-6678-46D7-A6BB-E914203A211B}" name="#"/>
+    <tableColumn id="2" xr3:uid="{38419638-DCB3-4890-9F22-0BB9BE085A84}" name="Hotel Name"/>
+    <tableColumn id="3" xr3:uid="{AA8A40EC-626F-43A9-BADB-3CE732E13F43}" name="Key"/>
+    <tableColumn id="4" xr3:uid="{224E2D53-F79C-4E23-92BB-D6B5272A2F0A}" name="URL"/>
+    <tableColumn id="5" xr3:uid="{BDF71282-2772-4972-9690-6A841B00E336}" name="Type"/>
+    <tableColumn id="6" xr3:uid="{0D95BAB7-AA65-4B8B-9A3E-144235740C84}" name="Rating"/>
+    <tableColumn id="7" xr3:uid="{3390F89B-0FEA-498F-8E7D-62C367AD40DB}" name="Reviews"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -10361,7 +10402,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G1109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A703" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C215" sqref="C215"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -10370,7 +10413,8 @@
     <col min="3" max="3" width="49.7109375" customWidth="1"/>
     <col min="4" max="4" width="80" customWidth="1"/>
     <col min="5" max="5" width="20" customWidth="1"/>
-    <col min="6" max="7" width="10" customWidth="1"/>
+    <col min="6" max="6" width="10" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -35882,5 +35926,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>